<commit_message>
revised pinout for 81-4 board
Signed-off-by: mk_e <mark@gemellocattivo.com>
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19995" windowHeight="7425"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="MPC5634 176LQFP OEM (81oemSZ)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="449">
   <si>
     <t>PIN</t>
   </si>
@@ -1247,13 +1247,127 @@
   </si>
   <si>
     <t>COOLANT_TEMP_I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cam </t>
+  </si>
+  <si>
+    <t>Crank</t>
+  </si>
+  <si>
+    <t>injector 4</t>
+  </si>
+  <si>
+    <t>injector 3</t>
+  </si>
+  <si>
+    <t>injector 2</t>
+  </si>
+  <si>
+    <t>injector 1</t>
+  </si>
+  <si>
+    <t>injector 5</t>
+  </si>
+  <si>
+    <t>injector 6</t>
+  </si>
+  <si>
+    <t>injector 7</t>
+  </si>
+  <si>
+    <t>injector 8</t>
+  </si>
+  <si>
+    <t>optional out 2</t>
+  </si>
+  <si>
+    <t>optional out 1</t>
+  </si>
+  <si>
+    <t>spark 1</t>
+  </si>
+  <si>
+    <t>spark 2</t>
+  </si>
+  <si>
+    <t>spark 4</t>
+  </si>
+  <si>
+    <t>spark 3</t>
+  </si>
+  <si>
+    <t>Coolant temp</t>
+  </si>
+  <si>
+    <t>TPS</t>
+  </si>
+  <si>
+    <t>MAF</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>EGT 2</t>
+  </si>
+  <si>
+    <t>EGT 1</t>
+  </si>
+  <si>
+    <t>WBO2 1</t>
+  </si>
+  <si>
+    <t>WBO2 2</t>
+  </si>
+  <si>
+    <t>Tilt sensor</t>
+  </si>
+  <si>
+    <t>intake temp</t>
+  </si>
+  <si>
+    <t>trans switch</t>
+  </si>
+  <si>
+    <t>intercooler a</t>
+  </si>
+  <si>
+    <t>intercooler b</t>
+  </si>
+  <si>
+    <t>Battery volt sensor</t>
+  </si>
+  <si>
+    <t>Barometric Pres</t>
+  </si>
+  <si>
+    <t>Gear a</t>
+  </si>
+  <si>
+    <t>gear b</t>
+  </si>
+  <si>
+    <t>gear c</t>
+  </si>
+  <si>
+    <t>fuel pump</t>
+  </si>
+  <si>
+    <t>fan 1</t>
+  </si>
+  <si>
+    <t>fan 2</t>
+  </si>
+  <si>
+    <t>common name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1507,7 +1621,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1550,6 +1664,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1645,7 +1762,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1680,7 +1796,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1856,17 +1971,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y185"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q83" sqref="Q83"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="22" max="22" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1928,11 +2046,14 @@
         <v>316</v>
       </c>
       <c r="U1" s="11"/>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="W1" s="27" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1943,11 +2064,11 @@
       <c r="S2" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="W2" s="26" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1958,11 +2079,11 @@
       <c r="S3" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="W3" s="26" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1976,11 +2097,11 @@
       <c r="T4" t="s">
         <v>352</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="W4" s="26" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1991,11 +2112,11 @@
       <c r="S5" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="W5" s="26" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2006,11 +2127,11 @@
       <c r="S6" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="V6" s="26" t="s">
+      <c r="W6" s="26" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2022,7 +2143,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2034,7 +2155,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2046,7 +2167,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2058,7 +2179,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2070,7 +2191,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2082,7 +2203,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2094,7 +2215,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2106,7 +2227,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2133,7 +2254,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2145,7 +2266,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2157,7 +2278,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2186,7 +2307,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2215,7 +2336,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2244,7 +2365,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2273,7 +2394,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2290,11 +2411,11 @@
       <c r="S22" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="V22" s="26" t="s">
+      <c r="W22" s="26" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2314,11 +2435,11 @@
       <c r="T23" t="s">
         <v>353</v>
       </c>
-      <c r="V23" s="26" t="s">
+      <c r="W23" s="26" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2336,7 +2457,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2354,7 +2475,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2378,7 +2499,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2399,7 +2520,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2423,7 +2544,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2444,7 +2565,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2456,7 +2577,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2476,11 +2597,11 @@
       <c r="T31" t="s">
         <v>355</v>
       </c>
-      <c r="V31" s="26" t="s">
+      <c r="W31" s="26" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2492,7 +2613,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2512,11 +2633,11 @@
       <c r="T33" t="s">
         <v>356</v>
       </c>
-      <c r="V33" s="26" t="s">
+      <c r="W33" s="26" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2528,7 +2649,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -2548,11 +2669,11 @@
       <c r="T35" t="s">
         <v>357</v>
       </c>
-      <c r="V35" s="26" t="s">
+      <c r="W35" s="26" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2572,11 +2693,11 @@
       <c r="T36" t="s">
         <v>358</v>
       </c>
-      <c r="V36" s="26" t="s">
+      <c r="W36" s="26" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -2594,7 +2715,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -2611,8 +2732,11 @@
       <c r="T38" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V38" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -2629,8 +2753,11 @@
       <c r="T39" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V39" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -2647,8 +2774,11 @@
       <c r="T40" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V40" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -2668,8 +2798,11 @@
       <c r="T41" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V41" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -2681,7 +2814,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -2701,8 +2834,11 @@
       <c r="T43" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -2714,7 +2850,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -2739,7 +2875,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -2764,7 +2900,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -2784,8 +2920,11 @@
       <c r="T47" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V47" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -2805,8 +2944,11 @@
       <c r="T48" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V48" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
       <c r="A49" s="12">
         <v>48</v>
       </c>
@@ -2823,8 +2965,11 @@
       <c r="T49" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V49" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
       <c r="A50" s="12">
         <v>49</v>
       </c>
@@ -2841,8 +2986,11 @@
       <c r="T50" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V50" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
       <c r="A51" s="12">
         <v>50</v>
       </c>
@@ -2859,8 +3007,11 @@
       <c r="T51" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V51" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -2880,8 +3031,11 @@
       <c r="T52" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V52" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23">
       <c r="A53" s="12">
         <v>52</v>
       </c>
@@ -2902,7 +3056,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -2920,7 +3074,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23">
       <c r="A55" s="12">
         <v>54</v>
       </c>
@@ -2938,7 +3092,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23">
       <c r="A56" s="12">
         <v>55</v>
       </c>
@@ -2950,7 +3104,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -2965,7 +3119,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -2977,7 +3131,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23">
       <c r="A59" s="12">
         <v>58</v>
       </c>
@@ -2992,7 +3146,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -3007,7 +3161,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -3024,11 +3178,14 @@
       <c r="T61" t="s">
         <v>372</v>
       </c>
-      <c r="V61" s="26" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V61" t="s">
+        <v>411</v>
+      </c>
+      <c r="W61" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23">
       <c r="A62" s="12">
         <v>61</v>
       </c>
@@ -3045,11 +3202,14 @@
       <c r="T62" t="s">
         <v>373</v>
       </c>
-      <c r="V62" s="26" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>412</v>
+      </c>
+      <c r="W62" s="26" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23">
       <c r="A63" s="12">
         <v>62</v>
       </c>
@@ -3061,7 +3221,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23">
       <c r="A64" s="12">
         <v>63</v>
       </c>
@@ -3078,11 +3238,11 @@
       <c r="S64" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="V64" s="26" t="s">
+      <c r="W64" s="26" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23">
       <c r="A65" s="12">
         <v>64</v>
       </c>
@@ -3100,7 +3260,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23">
       <c r="A66" s="12">
         <v>65</v>
       </c>
@@ -3120,11 +3280,11 @@
       <c r="T66" t="s">
         <v>374</v>
       </c>
-      <c r="V66" s="26" t="s">
+      <c r="W66" s="26" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23">
       <c r="A67" s="12">
         <v>66</v>
       </c>
@@ -3149,7 +3309,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23">
       <c r="A68" s="12">
         <v>67</v>
       </c>
@@ -3169,11 +3329,11 @@
       <c r="T68" t="s">
         <v>375</v>
       </c>
-      <c r="V68" s="26" t="s">
+      <c r="W68" s="26" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23">
       <c r="A69" s="12">
         <v>68</v>
       </c>
@@ -3198,7 +3358,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23">
       <c r="A70" s="12">
         <v>69</v>
       </c>
@@ -3223,7 +3383,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23">
       <c r="A71" s="12">
         <v>70</v>
       </c>
@@ -3245,11 +3405,14 @@
       <c r="T71" t="s">
         <v>376</v>
       </c>
-      <c r="V71" s="26" t="s">
+      <c r="V71" t="s">
+        <v>421</v>
+      </c>
+      <c r="W71" s="26" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23">
       <c r="A72" s="12">
         <v>71</v>
       </c>
@@ -3271,11 +3434,14 @@
       <c r="T72" t="s">
         <v>377</v>
       </c>
-      <c r="V72" s="26" t="s">
+      <c r="V72" t="s">
+        <v>422</v>
+      </c>
+      <c r="W72" s="26" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23">
       <c r="A73" s="12">
         <v>72</v>
       </c>
@@ -3287,7 +3453,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23">
       <c r="A74" s="12">
         <v>73</v>
       </c>
@@ -3304,11 +3470,11 @@
       <c r="T74" t="s">
         <v>378</v>
       </c>
-      <c r="V74" s="26" t="s">
+      <c r="W74" s="26" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23">
       <c r="A75" s="12">
         <v>74</v>
       </c>
@@ -3320,7 +3486,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23">
       <c r="A76" s="12">
         <v>75</v>
       </c>
@@ -3334,11 +3500,11 @@
       <c r="S76" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="V76" s="26" t="s">
+      <c r="W76" s="26" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23">
       <c r="A77" s="12">
         <v>76</v>
       </c>
@@ -3358,11 +3524,11 @@
       <c r="S77" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="V77" s="26" t="s">
+      <c r="W77" s="26" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23">
       <c r="A78" s="12">
         <v>77</v>
       </c>
@@ -3379,8 +3545,11 @@
       <c r="T78" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V78" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23">
       <c r="A79" s="12">
         <v>78</v>
       </c>
@@ -3403,8 +3572,11 @@
       <c r="T79" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V79" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23">
       <c r="A80" s="12">
         <v>79</v>
       </c>
@@ -3424,8 +3596,11 @@
       <c r="T80" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V80" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23">
       <c r="A81" s="12">
         <v>80</v>
       </c>
@@ -3442,8 +3617,11 @@
       <c r="T81" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V81" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23">
       <c r="A82" s="12">
         <v>81</v>
       </c>
@@ -3463,11 +3641,11 @@
       <c r="U82" t="s">
         <v>315</v>
       </c>
-      <c r="V82" s="26" t="s">
+      <c r="W82" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23">
       <c r="A83" s="12">
         <v>82</v>
       </c>
@@ -3487,11 +3665,11 @@
       <c r="U83" t="s">
         <v>315</v>
       </c>
-      <c r="V83" s="26" t="s">
+      <c r="W83" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23">
       <c r="A84" s="12">
         <v>83</v>
       </c>
@@ -3512,7 +3690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23">
       <c r="A85" s="12">
         <v>84</v>
       </c>
@@ -3525,11 +3703,11 @@
       <c r="S85" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="V85" s="26" t="s">
+      <c r="W85" s="26" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23">
       <c r="A86" s="12">
         <v>85</v>
       </c>
@@ -3550,7 +3728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23">
       <c r="A87" s="12">
         <v>86</v>
       </c>
@@ -3571,7 +3749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23">
       <c r="A88" s="12">
         <v>87</v>
       </c>
@@ -3584,11 +3762,11 @@
       <c r="S88" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="V88" s="26" t="s">
+      <c r="W88" s="26" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23">
       <c r="A89" s="12">
         <v>88</v>
       </c>
@@ -3613,7 +3791,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23">
       <c r="A90" s="12">
         <v>89</v>
       </c>
@@ -3638,7 +3816,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23">
       <c r="A91" s="12">
         <v>90</v>
       </c>
@@ -3650,7 +3828,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23">
       <c r="A92" s="12">
         <v>91</v>
       </c>
@@ -3662,7 +3840,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23">
       <c r="A93" s="12">
         <v>92</v>
       </c>
@@ -3674,7 +3852,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23">
       <c r="A94" s="12">
         <v>93</v>
       </c>
@@ -3686,7 +3864,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23">
       <c r="A95" s="12">
         <v>94</v>
       </c>
@@ -3698,7 +3876,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23">
       <c r="A96" s="12">
         <v>95</v>
       </c>
@@ -3710,7 +3888,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23">
       <c r="A97" s="12">
         <v>96</v>
       </c>
@@ -3722,7 +3900,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23">
       <c r="A98" s="12">
         <v>97</v>
       </c>
@@ -3734,7 +3912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23">
       <c r="A99" s="12">
         <v>98</v>
       </c>
@@ -3755,7 +3933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23">
       <c r="A100" s="12">
         <v>99</v>
       </c>
@@ -3775,11 +3953,11 @@
       <c r="T100" t="s">
         <v>315</v>
       </c>
-      <c r="V100" s="26" t="s">
+      <c r="W100" s="26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23">
       <c r="A101" s="12">
         <v>100</v>
       </c>
@@ -3799,11 +3977,11 @@
       <c r="T101" t="s">
         <v>315</v>
       </c>
-      <c r="V101" s="26" t="s">
+      <c r="W101" s="26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23">
       <c r="A102" s="12">
         <v>101</v>
       </c>
@@ -3824,7 +4002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23">
       <c r="A103" s="12">
         <v>102</v>
       </c>
@@ -3836,7 +4014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23">
       <c r="A104" s="12">
         <v>103</v>
       </c>
@@ -3848,7 +4026,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23">
       <c r="A105" s="12">
         <v>104</v>
       </c>
@@ -3868,11 +4046,11 @@
       <c r="T105" t="s">
         <v>383</v>
       </c>
-      <c r="V105" s="26" t="s">
+      <c r="W105" s="26" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23">
       <c r="A106" s="12">
         <v>105</v>
       </c>
@@ -3893,7 +4071,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23">
       <c r="A107" s="12">
         <v>106</v>
       </c>
@@ -3914,7 +4092,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23">
       <c r="A108" s="12">
         <v>107</v>
       </c>
@@ -3932,7 +4110,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23">
       <c r="A109" s="12">
         <v>108</v>
       </c>
@@ -3944,7 +4122,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23">
       <c r="A110" s="12">
         <v>109</v>
       </c>
@@ -3959,7 +4137,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23">
       <c r="A111" s="12">
         <v>110</v>
       </c>
@@ -3971,7 +4149,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23">
       <c r="A112" s="12">
         <v>111</v>
       </c>
@@ -3985,11 +4163,11 @@
       <c r="S112" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="V112" s="26" t="s">
+      <c r="W112" s="26" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20">
       <c r="A113" s="12">
         <v>112</v>
       </c>
@@ -4010,7 +4188,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20">
       <c r="A114" s="12">
         <v>113</v>
       </c>
@@ -4031,7 +4209,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20">
       <c r="A115" s="12">
         <v>114</v>
       </c>
@@ -4052,7 +4230,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20">
       <c r="A116" s="12">
         <v>115</v>
       </c>
@@ -4064,7 +4242,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20">
       <c r="A117" s="12">
         <v>116</v>
       </c>
@@ -4093,7 +4271,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20">
       <c r="A118" s="12">
         <v>117</v>
       </c>
@@ -4122,7 +4300,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20">
       <c r="A119" s="12">
         <v>118</v>
       </c>
@@ -4151,7 +4329,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20">
       <c r="A120" s="12">
         <v>119</v>
       </c>
@@ -4163,7 +4341,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20">
       <c r="A121" s="12">
         <v>120</v>
       </c>
@@ -4190,7 +4368,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20">
       <c r="A122" s="12">
         <v>121</v>
       </c>
@@ -4202,7 +4380,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20">
       <c r="A123" s="12">
         <v>122</v>
       </c>
@@ -4217,7 +4395,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20">
       <c r="A124" s="12">
         <v>123</v>
       </c>
@@ -4235,7 +4413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20">
       <c r="A125" s="12">
         <v>124</v>
       </c>
@@ -4253,7 +4431,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20">
       <c r="A126" s="12">
         <v>125</v>
       </c>
@@ -4265,7 +4443,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20">
       <c r="A127" s="12">
         <v>126</v>
       </c>
@@ -4283,7 +4461,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20">
       <c r="A128" s="12">
         <v>127</v>
       </c>
@@ -4295,7 +4473,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23">
       <c r="A129" s="12">
         <v>128</v>
       </c>
@@ -4307,7 +4485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23">
       <c r="A130" s="12">
         <v>129</v>
       </c>
@@ -4325,7 +4503,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23">
       <c r="A131" s="12">
         <v>130</v>
       </c>
@@ -4343,7 +4521,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23">
       <c r="A132" s="12">
         <v>131</v>
       </c>
@@ -4355,7 +4533,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23">
       <c r="A133" s="12">
         <v>132</v>
       </c>
@@ -4380,7 +4558,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23">
       <c r="A134" s="12">
         <v>133</v>
       </c>
@@ -4392,7 +4570,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23">
       <c r="A135" s="12">
         <v>134</v>
       </c>
@@ -4409,9 +4587,9 @@
       <c r="S135" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="V135" s="26"/>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W135" s="26"/>
+    </row>
+    <row r="136" spans="1:23">
       <c r="A136" s="12">
         <v>135</v>
       </c>
@@ -4428,9 +4606,9 @@
       <c r="S136" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="V136" s="26"/>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W136" s="26"/>
+    </row>
+    <row r="137" spans="1:23">
       <c r="A137" s="12">
         <v>136</v>
       </c>
@@ -4447,9 +4625,9 @@
       <c r="S137" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="V137" s="26"/>
-    </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W137" s="26"/>
+    </row>
+    <row r="138" spans="1:23">
       <c r="A138" s="12">
         <v>137</v>
       </c>
@@ -4466,9 +4644,9 @@
       <c r="S138" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="V138" s="26"/>
-    </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W138" s="26"/>
+    </row>
+    <row r="139" spans="1:23">
       <c r="A139" s="12">
         <v>138</v>
       </c>
@@ -4480,7 +4658,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23">
       <c r="A140" s="12">
         <v>139</v>
       </c>
@@ -4498,7 +4676,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23">
       <c r="A141" s="12">
         <v>140</v>
       </c>
@@ -4510,7 +4688,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23">
       <c r="A142" s="12">
         <v>141</v>
       </c>
@@ -4522,7 +4700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23">
       <c r="A143" s="12">
         <v>142</v>
       </c>
@@ -4536,8 +4714,11 @@
       <c r="T143" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V143" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23">
       <c r="A144" s="12">
         <v>143</v>
       </c>
@@ -4551,8 +4732,11 @@
       <c r="T144" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V144" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23">
       <c r="A145" s="12">
         <v>144</v>
       </c>
@@ -4566,8 +4750,11 @@
       <c r="T145" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V145" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23">
       <c r="A146" s="12">
         <v>145</v>
       </c>
@@ -4581,11 +4768,11 @@
       <c r="S146" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="V146" s="26" t="s">
+      <c r="W146" s="26" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23">
       <c r="A147" s="12">
         <v>146</v>
       </c>
@@ -4599,11 +4786,11 @@
       <c r="S147" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="V147" s="26" t="s">
+      <c r="W147" s="26" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23">
       <c r="A148" s="12">
         <v>147</v>
       </c>
@@ -4617,11 +4804,11 @@
       <c r="S148" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="V148" s="26" t="s">
+      <c r="W148" s="26" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23">
       <c r="A149" s="12">
         <v>148</v>
       </c>
@@ -4635,11 +4822,11 @@
       <c r="S149" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="V149" s="26" t="s">
+      <c r="W149" s="26" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23">
       <c r="A150" s="12">
         <v>149</v>
       </c>
@@ -4651,7 +4838,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23">
       <c r="A151" s="12">
         <v>150</v>
       </c>
@@ -4662,11 +4849,11 @@
       <c r="S151" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="V151" s="26" t="s">
+      <c r="W151" s="26" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23">
       <c r="A152" s="12">
         <v>151</v>
       </c>
@@ -4680,8 +4867,11 @@
       <c r="T152" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V152" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="153" spans="1:23">
       <c r="A153" s="12">
         <v>152</v>
       </c>
@@ -4693,7 +4883,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23">
       <c r="A154" s="12">
         <v>153</v>
       </c>
@@ -4708,7 +4898,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23">
       <c r="A155" s="12">
         <v>154</v>
       </c>
@@ -4723,7 +4913,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23">
       <c r="A156" s="12">
         <v>155</v>
       </c>
@@ -4738,7 +4928,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23">
       <c r="A157" s="12">
         <v>156</v>
       </c>
@@ -4753,7 +4943,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23">
       <c r="A158" s="12">
         <v>157</v>
       </c>
@@ -4767,8 +4957,11 @@
       <c r="T158" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V158" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="159" spans="1:23">
       <c r="A159" s="12">
         <v>158</v>
       </c>
@@ -4782,8 +4975,11 @@
       <c r="T159" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V159" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="160" spans="1:23">
       <c r="A160" s="12">
         <v>159</v>
       </c>
@@ -4797,8 +4993,11 @@
       <c r="T160" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V160" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="161" spans="1:23">
       <c r="A161" s="12">
         <v>160</v>
       </c>
@@ -4812,8 +5011,11 @@
       <c r="T161" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V161" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="162" spans="1:23">
       <c r="A162" s="12">
         <v>161</v>
       </c>
@@ -4827,8 +5029,11 @@
       <c r="T162" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V162" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="163" spans="1:23">
       <c r="A163" s="12">
         <v>162</v>
       </c>
@@ -4840,7 +5045,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23">
       <c r="A164" s="12">
         <v>163</v>
       </c>
@@ -4852,7 +5057,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23">
       <c r="A165" s="12">
         <v>164</v>
       </c>
@@ -4864,7 +5069,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23">
       <c r="A166" s="12">
         <v>165</v>
       </c>
@@ -4878,11 +5083,14 @@
       <c r="T166" t="s">
         <v>402</v>
       </c>
-      <c r="V166" s="26" t="s">
+      <c r="V166" t="s">
+        <v>435</v>
+      </c>
+      <c r="W166" s="26" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23">
       <c r="A167" s="12">
         <v>166</v>
       </c>
@@ -4896,11 +5104,14 @@
       <c r="T167" t="s">
         <v>403</v>
       </c>
-      <c r="V167" s="26" t="s">
+      <c r="V167" t="s">
+        <v>434</v>
+      </c>
+      <c r="W167" s="26" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23">
       <c r="A168" s="12">
         <v>167</v>
       </c>
@@ -4914,11 +5125,14 @@
       <c r="T168" t="s">
         <v>404</v>
       </c>
-      <c r="V168" s="26" t="s">
+      <c r="V168" t="s">
+        <v>433</v>
+      </c>
+      <c r="W168" s="26" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23">
       <c r="A169" s="12">
         <v>168</v>
       </c>
@@ -4932,11 +5146,14 @@
       <c r="T169" t="s">
         <v>405</v>
       </c>
-      <c r="V169" s="26" t="s">
+      <c r="V169" t="s">
+        <v>432</v>
+      </c>
+      <c r="W169" s="26" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23">
       <c r="A170" s="12">
         <v>169</v>
       </c>
@@ -4950,11 +5167,14 @@
       <c r="T170" t="s">
         <v>406</v>
       </c>
-      <c r="V170" s="26" t="s">
+      <c r="V170" t="s">
+        <v>431</v>
+      </c>
+      <c r="W170" s="26" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23">
       <c r="A171" s="12">
         <v>170</v>
       </c>
@@ -4968,11 +5188,14 @@
       <c r="T171" t="s">
         <v>407</v>
       </c>
-      <c r="V171" s="26" t="s">
+      <c r="V171" t="s">
+        <v>430</v>
+      </c>
+      <c r="W171" s="26" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23">
       <c r="A172" s="12">
         <v>171</v>
       </c>
@@ -4986,11 +5209,14 @@
       <c r="T172" t="s">
         <v>408</v>
       </c>
-      <c r="V172" s="26" t="s">
+      <c r="V172" t="s">
+        <v>429</v>
+      </c>
+      <c r="W172" s="26" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23">
       <c r="A173" s="12">
         <v>172</v>
       </c>
@@ -5004,11 +5230,14 @@
       <c r="T173" t="s">
         <v>409</v>
       </c>
-      <c r="V173" s="26" t="s">
+      <c r="V173" t="s">
+        <v>428</v>
+      </c>
+      <c r="W173" s="26" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23">
       <c r="A174" s="12">
         <v>173</v>
       </c>
@@ -5022,8 +5251,11 @@
       <c r="T174" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V174" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23">
       <c r="A175" s="12">
         <v>174</v>
       </c>
@@ -5035,7 +5267,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23">
       <c r="A176" s="12">
         <v>175</v>
       </c>
@@ -5047,7 +5279,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="177" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:26" ht="15.75" thickBot="1">
       <c r="A177" s="7">
         <v>176</v>
       </c>
@@ -5072,10 +5304,10 @@
         <v>288</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:26">
       <c r="T179" s="24"/>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:26">
       <c r="R180" t="s">
         <v>294</v>
       </c>
@@ -5092,8 +5324,9 @@
       <c r="W180" s="24"/>
       <c r="X180" s="24"/>
       <c r="Y180" s="24"/>
-    </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z180" s="24"/>
+    </row>
+    <row r="181" spans="1:26">
       <c r="S181" t="s">
         <v>296</v>
       </c>
@@ -5101,7 +5334,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:26">
       <c r="S182" t="s">
         <v>298</v>
       </c>
@@ -5109,7 +5342,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:26">
       <c r="R184" t="s">
         <v>300</v>
       </c>
@@ -5117,7 +5350,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:26">
       <c r="S185" t="s">
         <v>293</v>
       </c>

</xml_diff>